<commit_message>
modified:   README.md 	modified:   design/test.xlsx
</commit_message>
<xml_diff>
--- a/design/test.xlsx
+++ b/design/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrls\OneDrive\学校事务\第四学期\综合应用\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrls\Documents\repo\nblog\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="21600" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -545,64 +545,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -618,26 +572,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,7 +876,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -934,7 +888,7 @@
     <col min="5" max="5" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -966,7 +920,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -981,7 +935,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -996,7 +950,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1011,7 +965,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1026,7 +980,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1041,7 +995,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1056,7 +1010,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1071,7 +1025,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1081,10 +1035,10 @@
       <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1099,7 +1053,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1114,7 +1068,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1129,7 +1083,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1144,7 +1098,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1157,9 +1111,9 @@
       <c r="D15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1174,7 +1128,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1189,7 +1143,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1204,7 +1158,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1219,7 +1173,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1234,7 +1188,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1249,7 +1203,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1264,7 +1218,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1279,7 +1233,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1294,7 +1248,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1309,7 +1263,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1324,7 +1278,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1339,7 +1293,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1354,7 +1308,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1369,7 +1323,7 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1384,7 +1338,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1399,55 +1353,59 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>33</v>
       </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>